<commit_message>
Added bulk account creation
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sir_m\quiz_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D163300-E0D8-4D11-919D-35054041C6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06A7C3-1FFA-4937-88CF-B6408D08D90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="142">
   <si>
     <t>Question</t>
   </si>
@@ -40,165 +40,428 @@
     <t>CorrectOp</t>
   </si>
   <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
     <t>What is the time complexity of binary search?</t>
   </si>
   <si>
+    <t>Which data structure works on FIFO?</t>
+  </si>
+  <si>
+    <t>Which protocol is used for web browsing?</t>
+  </si>
+  <si>
+    <t>Which logic gate outputs 1 when both inputs are 1?</t>
+  </si>
+  <si>
+    <t>What does CPU stand for?</t>
+  </si>
+  <si>
+    <t>Which language is object-oriented?</t>
+  </si>
+  <si>
+    <t>Which component stores data permanently?</t>
+  </si>
+  <si>
+    <t>What is the extension of Python files?</t>
+  </si>
+  <si>
+    <t>Which of these is a relational database?</t>
+  </si>
+  <si>
+    <t>Which device converts digital signals to analog?</t>
+  </si>
+  <si>
+    <t>Which data structure uses LIFO order?</t>
+  </si>
+  <si>
+    <t>What is the time complexity of merge sort?</t>
+  </si>
+  <si>
+    <t>Which of the following is not a linear data structure?</t>
+  </si>
+  <si>
+    <t>What is the best case time complexity of quick sort?</t>
+  </si>
+  <si>
+    <t>Which data structure is used for recursion?</t>
+  </si>
+  <si>
+    <t>Which traversal is used in Depth First Search?</t>
+  </si>
+  <si>
+    <t>Which of the following sorting algorithms is stable?</t>
+  </si>
+  <si>
+    <t>What is the space complexity of bubble sort?</t>
+  </si>
+  <si>
+    <t>Which of these is an application of stack?</t>
+  </si>
+  <si>
+    <t>Which tree is always height-balanced?</t>
+  </si>
+  <si>
+    <t>Which data structure is used in BFS?</t>
+  </si>
+  <si>
+    <t>Which algorithm is used to find shortest paths in graphs?</t>
+  </si>
+  <si>
+    <t>Which hashing technique handles collisions using linked lists?</t>
+  </si>
+  <si>
+    <t>Which of the following is not an example of Divide and Conquer?</t>
+  </si>
+  <si>
+    <t>What is the worst case time complexity of binary search?</t>
+  </si>
+  <si>
+    <t>Which of the following is used in priority queues?</t>
+  </si>
+  <si>
+    <t>What is the in-order traversal of a binary search tree used for?</t>
+  </si>
+  <si>
+    <t>What is the maximum number of nodes in a binary tree of height h?</t>
+  </si>
+  <si>
+    <t>Which operation is not possible in O(1) in a stack?</t>
+  </si>
+  <si>
+    <t>Which data structure uses key-value pairs?</t>
+  </si>
+  <si>
+    <t>Which traversal method uses recursion naturally?</t>
+  </si>
+  <si>
+    <t>Which of these is not a tree traversal method?</t>
+  </si>
+  <si>
+    <t>Which sorting algorithm is best for nearly sorted data?</t>
+  </si>
+  <si>
+    <t>Which algorithm is used to detect cycles in a directed graph?</t>
+  </si>
+  <si>
+    <t>What is the auxiliary space of merge sort?</t>
+  </si>
+  <si>
+    <t>Which data structure can be used to implement recursion iteratively?</t>
+  </si>
+  <si>
+    <t>Which operation is faster in a linked list compared to an array?</t>
+  </si>
+  <si>
+    <t>What is the main advantage of a doubly linked list over singly linked list?</t>
+  </si>
+  <si>
+    <t>Which graph traversal uses a queue?</t>
+  </si>
+  <si>
     <t>O(n)</t>
   </si>
   <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Central Process Unit</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>O(n log n)</t>
+  </si>
+  <si>
+    <t>Level Order</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Job Scheduling</t>
+  </si>
+  <si>
+    <t>Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Prim’s</t>
+  </si>
+  <si>
+    <t>Chaining</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>2^h - 1</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Inorder</t>
+  </si>
+  <si>
+    <t>Insertion Sort</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>Random Access</t>
+  </si>
+  <si>
+    <t>Less Memory</t>
+  </si>
+  <si>
     <t>O(log n)</t>
   </si>
   <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>Core Processing Utility</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>.py</t>
+  </si>
+  <si>
+    <t>Redis</t>
+  </si>
+  <si>
+    <t>Modem</t>
+  </si>
+  <si>
     <t>O(n^2)</t>
   </si>
   <si>
-    <t>O(1)</t>
-  </si>
-  <si>
-    <t>Which data structure works on FIFO?</t>
-  </si>
-  <si>
-    <t>Stack</t>
-  </si>
-  <si>
-    <t>Queue</t>
+    <t>Postorder</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>AVL Tree</t>
+  </si>
+  <si>
+    <t>Dijkstra’s</t>
+  </si>
+  <si>
+    <t>Open Addressing</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>2^(h+1) - 1</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Faster Access</t>
   </si>
   <si>
     <t>Tree</t>
   </si>
   <si>
+    <t>SMTP</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Central Processing Unit</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>.java</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
     <t>Graph</t>
   </si>
   <si>
-    <t>Which protocol is used for web browsing?</t>
-  </si>
-  <si>
-    <t>HTTP</t>
-  </si>
-  <si>
-    <t>FTP</t>
-  </si>
-  <si>
-    <t>SMTP</t>
+    <t>Heap Sort</t>
+  </si>
+  <si>
+    <t>Routing</t>
+  </si>
+  <si>
+    <t>B-Tree</t>
+  </si>
+  <si>
+    <t>Kruskal’s</t>
+  </si>
+  <si>
+    <t>Probing</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>h^2</t>
+  </si>
+  <si>
+    <t>Peek</t>
+  </si>
+  <si>
+    <t>Hash Table</t>
+  </si>
+  <si>
+    <t>Preorder</t>
+  </si>
+  <si>
+    <t>Reverseorder</t>
+  </si>
+  <si>
+    <t>Bubble Sort</t>
+  </si>
+  <si>
+    <t>Kruskal</t>
+  </si>
+  <si>
+    <t>Backward Traversal</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
   </si>
   <si>
     <t>SSH</t>
   </si>
   <si>
-    <t>Which logic gate outputs 1 when both inputs are 1?</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>XOR</t>
-  </si>
-  <si>
-    <t>AND</t>
-  </si>
-  <si>
     <t>NAND</t>
   </si>
   <si>
-    <t>What does CPU stand for?</t>
-  </si>
-  <si>
-    <t>Central Process Unit</t>
-  </si>
-  <si>
-    <t>Core Processing Utility</t>
-  </si>
-  <si>
-    <t>Central Processing Unit</t>
-  </si>
-  <si>
     <t>Compute Power Unit</t>
   </si>
   <si>
-    <t>Which language is object-oriented?</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Assembly</t>
-  </si>
-  <si>
     <t>HTML</t>
   </si>
   <si>
-    <t>Which component stores data permanently?</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>ROM</t>
-  </si>
-  <si>
-    <t>Cache</t>
-  </si>
-  <si>
     <t>Registers</t>
   </si>
   <si>
-    <t>What is the extension of Python files?</t>
-  </si>
-  <si>
-    <t>.txt</t>
-  </si>
-  <si>
-    <t>.py</t>
-  </si>
-  <si>
-    <t>.java</t>
-  </si>
-  <si>
     <t>.exe</t>
   </si>
   <si>
-    <t>Which of these is a relational database?</t>
-  </si>
-  <si>
-    <t>MongoDB</t>
-  </si>
-  <si>
-    <t>Redis</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
     <t>Neo4j</t>
   </si>
   <si>
-    <t>Which device converts digital signals to analog?</t>
-  </si>
-  <si>
-    <t>Router</t>
-  </si>
-  <si>
-    <t>Modem</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
     <t>Repeater</t>
   </si>
   <si>
-    <t>Difficulty</t>
+    <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>Paging</t>
+  </si>
+  <si>
+    <t>Threaded Tree</t>
+  </si>
+  <si>
+    <t>Floyd’s</t>
+  </si>
+  <si>
+    <t>Rehashing</t>
+  </si>
+  <si>
+    <t>Balancing</t>
+  </si>
+  <si>
+    <t>log(h)</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Prim</t>
+  </si>
+  <si>
+    <t>Indexing</t>
+  </si>
+  <si>
+    <t>Bellman-Ford</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -214,7 +477,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -222,12 +485,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,9 +527,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -286,7 +567,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -320,6 +601,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -354,9 +636,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,63 +813,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>56</v>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -594,22 +876,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -617,22 +899,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G4">
         <v>13</v>
@@ -640,22 +922,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -663,22 +945,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -686,42 +968,42 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -729,22 +1011,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -752,22 +1034,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -775,28 +1057,695 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>